<commit_message>
Bump catch carrier assy in part list, add friction clamp nut
</commit_message>
<xml_diff>
--- a/Part Listing.xlsx
+++ b/Part Listing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/642-MSED/AFL/AFL-hardware-devel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pab2/Documents/GitHub/AFL-hardware-devel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{322C69CD-E9BF-7741-A09A-EC9117A5C389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5460B8-5634-DD44-9E7E-6ADA1C541D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12300" yWindow="-22120" windowWidth="28040" windowHeight="17180" xr2:uid="{E437F38B-91C4-4D42-82D0-A114F0D947B5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26720" xr2:uid="{E437F38B-91C4-4D42-82D0-A114F0D947B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -285,9 +285,6 @@
     <t>AFL-101-001-02-1</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>ExternalComponents (002)</t>
   </si>
   <si>
@@ -550,6 +547,9 @@
   </si>
   <si>
     <t>AFL-101-006-02-1</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -609,13 +609,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,9 +633,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -674,7 +673,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -780,7 +779,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -922,7 +921,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -932,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2438C84-1458-8840-BF88-E04D5AA1BBCE}">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -971,7 +970,7 @@
         <v>3</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K1" t="s">
         <v>5</v>
@@ -997,8 +996,8 @@
       <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>150</v>
+      <c r="I3" t="s">
+        <v>149</v>
       </c>
       <c r="K3" t="s">
         <v>10</v>
@@ -1023,8 +1022,8 @@
       <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>150</v>
+      <c r="I4" t="s">
+        <v>149</v>
       </c>
       <c r="K4" t="s">
         <v>9</v>
@@ -1049,8 +1048,8 @@
       <c r="G5" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>149</v>
+      <c r="I5" t="s">
+        <v>148</v>
       </c>
       <c r="K5" t="s">
         <v>25</v>
@@ -1075,22 +1074,22 @@
       <c r="G6" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>149</v>
+      <c r="I6" t="s">
+        <v>148</v>
       </c>
       <c r="K6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I7" s="5"/>
+      <c r="I7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>170</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -1099,13 +1098,13 @@
         <v>76</v>
       </c>
       <c r="F8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G8" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>140</v>
+      <c r="I8" t="s">
+        <v>139</v>
       </c>
       <c r="K8" t="s">
         <v>12</v>
@@ -1113,7 +1112,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
         <v>40</v>
@@ -1125,13 +1124,13 @@
         <v>76</v>
       </c>
       <c r="F9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G9" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>141</v>
+      <c r="I9" t="s">
+        <v>140</v>
       </c>
       <c r="K9" t="s">
         <v>61</v>
@@ -1139,7 +1138,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
@@ -1151,19 +1150,19 @@
         <v>76</v>
       </c>
       <c r="F10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G10" t="s">
         <v>62</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10"/>
       <c r="K10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
         <v>31</v>
@@ -1175,22 +1174,22 @@
         <v>76</v>
       </c>
       <c r="F11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G11" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="5"/>
+      <c r="I11"/>
       <c r="K11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I12" s="5"/>
+      <c r="I12"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
@@ -1202,13 +1201,13 @@
         <v>76</v>
       </c>
       <c r="F13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G13" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="5" t="s">
-        <v>142</v>
+      <c r="I13" t="s">
+        <v>141</v>
       </c>
       <c r="K13" t="s">
         <v>26</v>
@@ -1216,7 +1215,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
         <v>40</v>
@@ -1228,22 +1227,22 @@
         <v>76</v>
       </c>
       <c r="F14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G14" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="5"/>
+      <c r="I14"/>
       <c r="K14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I15" s="5"/>
+      <c r="I15"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B16" t="s">
         <v>40</v>
@@ -1255,24 +1254,24 @@
         <v>76</v>
       </c>
       <c r="F16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G16" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>143</v>
+      <c r="I16" t="s">
+        <v>142</v>
       </c>
       <c r="K16" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I17" s="5"/>
+      <c r="I17"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
@@ -1284,16 +1283,16 @@
         <v>76</v>
       </c>
       <c r="F18" t="s">
+        <v>115</v>
+      </c>
+      <c r="G18" t="s">
         <v>116</v>
       </c>
-      <c r="G18" t="s">
-        <v>117</v>
-      </c>
-      <c r="I18" s="5"/>
+      <c r="I18"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B19" t="s">
         <v>40</v>
@@ -1305,16 +1304,16 @@
         <v>76</v>
       </c>
       <c r="F19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G19" t="s">
-        <v>118</v>
-      </c>
-      <c r="I19" s="5"/>
+        <v>117</v>
+      </c>
+      <c r="I19"/>
     </row>
     <row r="20" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B20" t="s">
         <v>40</v>
@@ -1326,110 +1325,110 @@
         <v>76</v>
       </c>
       <c r="F20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G20" t="s">
-        <v>119</v>
-      </c>
-      <c r="I20" s="5"/>
+        <v>118</v>
+      </c>
+      <c r="I20"/>
     </row>
     <row r="21" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I21" s="5"/>
+      <c r="I21"/>
     </row>
     <row r="22" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B22" t="s">
         <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E22" t="s">
         <v>76</v>
       </c>
       <c r="F22" t="s">
+        <v>159</v>
+      </c>
+      <c r="G22" t="s">
         <v>160</v>
       </c>
-      <c r="G22" t="s">
+      <c r="I22" t="s">
         <v>161</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B23" t="s">
         <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E23" t="s">
         <v>76</v>
       </c>
       <c r="F23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G23" t="s">
+        <v>164</v>
+      </c>
+      <c r="I23" t="s">
         <v>165</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B24" t="s">
         <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E24" t="s">
         <v>76</v>
       </c>
       <c r="F24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G24" t="s">
-        <v>168</v>
-      </c>
-      <c r="I24" s="5"/>
+        <v>167</v>
+      </c>
+      <c r="I24"/>
     </row>
     <row r="25" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B25" t="s">
         <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E25" t="s">
         <v>76</v>
       </c>
       <c r="F25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G25" t="s">
-        <v>169</v>
-      </c>
-      <c r="I25" s="5"/>
+        <v>168</v>
+      </c>
+      <c r="I25"/>
     </row>
     <row r="26" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I26" s="5"/>
+      <c r="I26"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B27" t="s">
         <v>40</v>
@@ -1438,16 +1437,16 @@
         <v>17</v>
       </c>
       <c r="E27" t="s">
+        <v>97</v>
+      </c>
+      <c r="F27" t="s">
         <v>98</v>
-      </c>
-      <c r="F27" t="s">
-        <v>99</v>
       </c>
       <c r="G27" t="s">
         <v>53</v>
       </c>
-      <c r="I27" s="5" t="s">
-        <v>145</v>
+      <c r="I27" t="s">
+        <v>144</v>
       </c>
       <c r="K27" t="s">
         <v>57</v>
@@ -1455,7 +1454,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
         <v>40</v>
@@ -1464,16 +1463,16 @@
         <v>17</v>
       </c>
       <c r="E28" t="s">
+        <v>97</v>
+      </c>
+      <c r="F28" t="s">
         <v>98</v>
-      </c>
-      <c r="F28" t="s">
-        <v>99</v>
       </c>
       <c r="G28" t="s">
         <v>54</v>
       </c>
-      <c r="I28" s="5" t="s">
-        <v>144</v>
+      <c r="I28" t="s">
+        <v>143</v>
       </c>
       <c r="K28" t="s">
         <v>58</v>
@@ -1481,7 +1480,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B29" t="s">
         <v>40</v>
@@ -1490,49 +1489,49 @@
         <v>17</v>
       </c>
       <c r="E29" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" t="s">
         <v>98</v>
-      </c>
-      <c r="F29" t="s">
-        <v>99</v>
       </c>
       <c r="G29" t="s">
         <v>55</v>
       </c>
-      <c r="I29" s="5"/>
+      <c r="I29"/>
       <c r="K29" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" t="s">
         <v>97</v>
       </c>
-      <c r="B30" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>98</v>
-      </c>
-      <c r="F30" t="s">
-        <v>99</v>
       </c>
       <c r="G30" t="s">
         <v>56</v>
       </c>
-      <c r="I30" s="5"/>
+      <c r="I30"/>
       <c r="K30" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I31" s="5"/>
+      <c r="I31"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B32" t="s">
         <v>40</v>
@@ -1541,21 +1540,21 @@
         <v>17</v>
       </c>
       <c r="E32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G32" t="s">
-        <v>137</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>146</v>
+        <v>136</v>
+      </c>
+      <c r="I32" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B33" t="s">
         <v>40</v>
@@ -1564,22 +1563,22 @@
         <v>17</v>
       </c>
       <c r="E33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G33" t="s">
-        <v>138</v>
-      </c>
-      <c r="I33" s="5"/>
+        <v>137</v>
+      </c>
+      <c r="I33"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I34" s="5"/>
+      <c r="I34"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
         <v>31</v>
@@ -1588,22 +1587,22 @@
         <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G35" t="s">
         <v>30</v>
       </c>
-      <c r="I35" s="5"/>
+      <c r="I35"/>
       <c r="K35" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B36" t="s">
         <v>40</v>
@@ -1612,25 +1611,25 @@
         <v>17</v>
       </c>
       <c r="E36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G36" t="s">
         <v>43</v>
       </c>
-      <c r="I36" s="5"/>
+      <c r="I36"/>
       <c r="K36" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I37" s="5"/>
+      <c r="I37"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B38" t="s">
         <v>63</v>
@@ -1639,22 +1638,22 @@
         <v>17</v>
       </c>
       <c r="E38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G38" t="s">
         <v>34</v>
       </c>
-      <c r="I38" s="5"/>
+      <c r="I38"/>
       <c r="K38" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
@@ -1663,22 +1662,22 @@
         <v>17</v>
       </c>
       <c r="E39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G39" t="s">
         <v>35</v>
       </c>
-      <c r="I39" s="5"/>
+      <c r="I39"/>
       <c r="K39" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B40" t="s">
         <v>63</v>
@@ -1687,22 +1686,22 @@
         <v>17</v>
       </c>
       <c r="E40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G40" t="s">
         <v>36</v>
       </c>
-      <c r="I40" s="5"/>
+      <c r="I40"/>
       <c r="K40" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B41" t="s">
         <v>40</v>
@@ -1711,25 +1710,25 @@
         <v>17</v>
       </c>
       <c r="E41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G41" t="s">
         <v>36</v>
       </c>
-      <c r="I41" s="5"/>
+      <c r="I41"/>
       <c r="K41" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I42" s="5"/>
+      <c r="I42"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B43" t="s">
         <v>63</v>
@@ -1738,22 +1737,22 @@
         <v>17</v>
       </c>
       <c r="E43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G43" t="s">
         <v>36</v>
       </c>
-      <c r="I43" s="5"/>
+      <c r="I43"/>
       <c r="K43" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B44" t="s">
         <v>31</v>
@@ -1762,25 +1761,25 @@
         <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G44" t="s">
+        <v>113</v>
+      </c>
+      <c r="I44"/>
+      <c r="K44" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="I44" s="5"/>
-      <c r="K44" s="3" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I45" s="5"/>
+      <c r="I45"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B46" t="s">
         <v>63</v>
@@ -1789,27 +1788,27 @@
         <v>17</v>
       </c>
       <c r="E46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G46" t="s">
         <v>41</v>
       </c>
-      <c r="I46" s="5" t="s">
-        <v>147</v>
+      <c r="I46" t="s">
+        <v>146</v>
       </c>
       <c r="K46" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I47" s="5"/>
+      <c r="I47"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B48" t="s">
         <v>40</v>
@@ -1818,16 +1817,16 @@
         <v>17</v>
       </c>
       <c r="E48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G48" t="s">
         <v>47</v>
       </c>
-      <c r="I48" s="5" t="s">
-        <v>148</v>
+      <c r="I48" t="s">
+        <v>147</v>
       </c>
       <c r="K48" t="s">
         <v>48</v>
@@ -1835,7 +1834,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B49" t="s">
         <v>40</v>
@@ -1844,25 +1843,25 @@
         <v>17</v>
       </c>
       <c r="E49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F49" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G49" t="s">
         <v>49</v>
       </c>
-      <c r="I49" s="5"/>
+      <c r="I49"/>
       <c r="K49" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I50" s="5"/>
+      <c r="I50"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B51" t="s">
         <v>40</v>
@@ -1871,25 +1870,25 @@
         <v>17</v>
       </c>
       <c r="E51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G51" t="s">
         <v>46</v>
       </c>
-      <c r="I51" s="5"/>
+      <c r="I51"/>
       <c r="K51" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I52" s="5"/>
+      <c r="I52"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B53" t="s">
         <v>40</v>
@@ -1898,25 +1897,25 @@
         <v>17</v>
       </c>
       <c r="E53" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F53" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G53" t="s">
         <v>52</v>
       </c>
-      <c r="I53" s="5"/>
+      <c r="I53"/>
       <c r="K53" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I54" s="5"/>
+      <c r="I54"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B55" t="s">
         <v>31</v>
@@ -1925,21 +1924,21 @@
         <v>17</v>
       </c>
       <c r="E55" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F55" t="s">
+        <v>151</v>
+      </c>
+      <c r="G55" t="s">
         <v>152</v>
       </c>
-      <c r="G55" t="s">
+      <c r="I55" t="s">
         <v>153</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B56" t="s">
         <v>31</v>
@@ -1948,24 +1947,24 @@
         <v>17</v>
       </c>
       <c r="E56" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F56" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G56" t="s">
-        <v>155</v>
-      </c>
-      <c r="I56" s="5" t="s">
         <v>154</v>
       </c>
+      <c r="I56" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I57" s="5"/>
+      <c r="I57"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B58" t="s">
         <v>40</v>
@@ -1974,17 +1973,17 @@
         <v>17</v>
       </c>
       <c r="E58" t="s">
+        <v>124</v>
+      </c>
+      <c r="F58" t="s">
         <v>125</v>
       </c>
-      <c r="F58" t="s">
+      <c r="G58" t="s">
         <v>126</v>
       </c>
-      <c r="G58" t="s">
+      <c r="I58"/>
+      <c r="K58" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="I58" s="5"/>
-      <c r="K58" s="3" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2070,12 +2069,12 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add substantial docs expansion
</commit_message>
<xml_diff>
--- a/Part Listing.xlsx
+++ b/Part Listing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pab2/Documents/GitHub/AFL-hardware-devel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5460B8-5634-DD44-9E7E-6ADA1C541D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655B5062-4A53-1949-84D8-0E47329A0DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26720" xr2:uid="{E437F38B-91C4-4D42-82D0-A114F0D947B5}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{E437F38B-91C4-4D42-82D0-A114F0D947B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="174">
   <si>
     <t>Part/Drawing ID</t>
   </si>
@@ -550,6 +550,15 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>AFL-101-002-01-4</t>
+  </si>
+  <si>
+    <t>Retainer nut</t>
+  </si>
+  <si>
+    <t>Tap hole 4-40</t>
   </si>
 </sst>
 </file>
@@ -929,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2438C84-1458-8840-BF88-E04D5AA1BBCE}">
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1185,40 +1194,37 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I12"/>
+      <c r="A12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" t="s">
+        <v>172</v>
+      </c>
+      <c r="I12" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F13" t="s">
-        <v>88</v>
-      </c>
-      <c r="G13" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" t="s">
-        <v>141</v>
-      </c>
-      <c r="K13" t="s">
-        <v>26</v>
-      </c>
+      <c r="I13"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -1230,69 +1236,74 @@
         <v>88</v>
       </c>
       <c r="G14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" t="s">
+        <v>141</v>
+      </c>
+      <c r="K14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" t="s">
         <v>29</v>
       </c>
-      <c r="I14"/>
-      <c r="K14" t="s">
+      <c r="I15"/>
+      <c r="K15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I15"/>
-    </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="I16"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>92</v>
       </c>
-      <c r="B16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
         <v>76</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F17" t="s">
         <v>89</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" t="s">
         <v>16</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I17" t="s">
         <v>142</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I17"/>
-    </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>119</v>
-      </c>
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" t="s">
-        <v>76</v>
-      </c>
-      <c r="F18" t="s">
-        <v>115</v>
-      </c>
-      <c r="G18" t="s">
-        <v>116</v>
-      </c>
       <c r="I18"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B19" t="s">
         <v>40</v>
@@ -1307,13 +1318,13 @@
         <v>115</v>
       </c>
       <c r="G19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I19"/>
     </row>
-    <row r="20" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B20" t="s">
         <v>40</v>
@@ -1328,39 +1339,37 @@
         <v>115</v>
       </c>
       <c r="G20" t="s">
+        <v>117</v>
+      </c>
+      <c r="I20"/>
+    </row>
+    <row r="21" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" t="s">
+        <v>115</v>
+      </c>
+      <c r="G21" t="s">
         <v>118</v>
       </c>
-      <c r="I20"/>
-    </row>
-    <row r="21" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I21"/>
     </row>
     <row r="22" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>162</v>
-      </c>
-      <c r="B22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" t="s">
-        <v>158</v>
-      </c>
-      <c r="E22" t="s">
-        <v>76</v>
-      </c>
-      <c r="F22" t="s">
-        <v>159</v>
-      </c>
-      <c r="G22" t="s">
-        <v>160</v>
-      </c>
-      <c r="I22" t="s">
-        <v>161</v>
-      </c>
+      <c r="I22"/>
     </row>
     <row r="23" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B23" t="s">
         <v>40</v>
@@ -1375,15 +1384,15 @@
         <v>159</v>
       </c>
       <c r="G23" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I23" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B24" t="s">
         <v>40</v>
@@ -1398,13 +1407,15 @@
         <v>159</v>
       </c>
       <c r="G24" t="s">
-        <v>167</v>
-      </c>
-      <c r="I24"/>
+        <v>164</v>
+      </c>
+      <c r="I24" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="25" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B25" t="s">
         <v>40</v>
@@ -1419,42 +1430,37 @@
         <v>159</v>
       </c>
       <c r="G25" t="s">
+        <v>167</v>
+      </c>
+      <c r="I25"/>
+    </row>
+    <row r="26" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>169</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>158</v>
+      </c>
+      <c r="E26" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" t="s">
+        <v>159</v>
+      </c>
+      <c r="G26" t="s">
         <v>168</v>
       </c>
-      <c r="I25"/>
-    </row>
-    <row r="26" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I26"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>93</v>
-      </c>
-      <c r="B27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" t="s">
-        <v>97</v>
-      </c>
-      <c r="F27" t="s">
-        <v>98</v>
-      </c>
-      <c r="G27" t="s">
-        <v>53</v>
-      </c>
-      <c r="I27" t="s">
-        <v>144</v>
-      </c>
-      <c r="K27" t="s">
-        <v>57</v>
-      </c>
+    <row r="27" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I27"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
         <v>40</v>
@@ -1469,18 +1475,18 @@
         <v>98</v>
       </c>
       <c r="G28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B29" t="s">
         <v>40</v>
@@ -1495,16 +1501,18 @@
         <v>98</v>
       </c>
       <c r="G29" t="s">
-        <v>55</v>
-      </c>
-      <c r="I29"/>
+        <v>54</v>
+      </c>
+      <c r="I29" t="s">
+        <v>143</v>
+      </c>
       <c r="K29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B30" t="s">
         <v>40</v>
@@ -1519,42 +1527,43 @@
         <v>98</v>
       </c>
       <c r="G30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I30"/>
       <c r="K30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" t="s">
+        <v>97</v>
+      </c>
+      <c r="F31" t="s">
+        <v>98</v>
+      </c>
+      <c r="G31" t="s">
+        <v>56</v>
+      </c>
+      <c r="I31"/>
+      <c r="K31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I31"/>
-    </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>134</v>
-      </c>
-      <c r="B32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" t="s">
-        <v>17</v>
-      </c>
-      <c r="E32" t="s">
-        <v>97</v>
-      </c>
-      <c r="F32" t="s">
-        <v>132</v>
-      </c>
-      <c r="G32" t="s">
-        <v>136</v>
-      </c>
-      <c r="I32" t="s">
-        <v>145</v>
-      </c>
+      <c r="I32"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B33" t="s">
         <v>40</v>
@@ -1569,43 +1578,42 @@
         <v>132</v>
       </c>
       <c r="G33" t="s">
+        <v>136</v>
+      </c>
+      <c r="I33" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" t="s">
+        <v>97</v>
+      </c>
+      <c r="F34" t="s">
+        <v>132</v>
+      </c>
+      <c r="G34" t="s">
         <v>137</v>
       </c>
-      <c r="I33"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I34"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>99</v>
-      </c>
-      <c r="B35" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" t="s">
-        <v>97</v>
-      </c>
-      <c r="F35" t="s">
-        <v>82</v>
-      </c>
-      <c r="G35" t="s">
-        <v>30</v>
-      </c>
       <c r="I35"/>
-      <c r="K35" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C36" t="s">
         <v>17</v>
@@ -1617,46 +1625,46 @@
         <v>82</v>
       </c>
       <c r="G36" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="I36"/>
       <c r="K36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" t="s">
+        <v>97</v>
+      </c>
+      <c r="F37" t="s">
+        <v>82</v>
+      </c>
+      <c r="G37" t="s">
+        <v>43</v>
+      </c>
+      <c r="I37"/>
+      <c r="K37" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I37"/>
-    </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>103</v>
-      </c>
-      <c r="B38" t="s">
-        <v>63</v>
-      </c>
-      <c r="C38" t="s">
-        <v>17</v>
-      </c>
-      <c r="E38" t="s">
-        <v>97</v>
-      </c>
-      <c r="F38" t="s">
-        <v>105</v>
-      </c>
-      <c r="G38" t="s">
-        <v>34</v>
-      </c>
       <c r="I38"/>
-      <c r="K38" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
@@ -1668,19 +1676,19 @@
         <v>105</v>
       </c>
       <c r="G39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I39"/>
       <c r="K39" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C40" t="s">
         <v>17</v>
@@ -1692,11 +1700,11 @@
         <v>105</v>
       </c>
       <c r="G40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I40"/>
       <c r="K40" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -1704,7 +1712,7 @@
         <v>101</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="C41" t="s">
         <v>17</v>
@@ -1720,42 +1728,42 @@
       </c>
       <c r="I41"/>
       <c r="K41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" t="s">
+        <v>97</v>
+      </c>
+      <c r="F42" t="s">
+        <v>105</v>
+      </c>
+      <c r="G42" t="s">
+        <v>36</v>
+      </c>
+      <c r="I42"/>
+      <c r="K42" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I42"/>
-    </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>104</v>
-      </c>
-      <c r="B43" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" t="s">
-        <v>17</v>
-      </c>
-      <c r="E43" t="s">
-        <v>97</v>
-      </c>
-      <c r="F43" t="s">
-        <v>106</v>
-      </c>
-      <c r="G43" t="s">
-        <v>36</v>
-      </c>
       <c r="I43"/>
-      <c r="K43" s="3" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B44" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="C44" t="s">
         <v>17</v>
@@ -1767,74 +1775,72 @@
         <v>106</v>
       </c>
       <c r="G44" t="s">
-        <v>113</v>
+        <v>36</v>
       </c>
       <c r="I44"/>
       <c r="K44" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" t="s">
+        <v>97</v>
+      </c>
+      <c r="F45" t="s">
+        <v>106</v>
+      </c>
+      <c r="G45" t="s">
+        <v>113</v>
+      </c>
+      <c r="I45"/>
+      <c r="K45" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I45"/>
-    </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="I46"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>108</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>63</v>
       </c>
-      <c r="C46" t="s">
-        <v>17</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="C47" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47" t="s">
         <v>97</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F47" t="s">
         <v>107</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G47" t="s">
         <v>41</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I47" t="s">
         <v>146</v>
       </c>
-      <c r="K46" t="s">
+      <c r="K47" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I47"/>
-    </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>130</v>
-      </c>
-      <c r="B48" t="s">
-        <v>40</v>
-      </c>
-      <c r="C48" t="s">
-        <v>17</v>
-      </c>
-      <c r="E48" t="s">
-        <v>122</v>
-      </c>
-      <c r="F48" t="s">
-        <v>133</v>
-      </c>
-      <c r="G48" t="s">
-        <v>47</v>
-      </c>
-      <c r="I48" t="s">
-        <v>147</v>
-      </c>
-      <c r="K48" t="s">
-        <v>48</v>
-      </c>
+      <c r="I48"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B49" t="s">
         <v>40</v>
@@ -1849,96 +1855,99 @@
         <v>133</v>
       </c>
       <c r="G49" t="s">
+        <v>47</v>
+      </c>
+      <c r="I49" t="s">
+        <v>147</v>
+      </c>
+      <c r="K49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>131</v>
+      </c>
+      <c r="B50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" t="s">
+        <v>122</v>
+      </c>
+      <c r="F50" t="s">
+        <v>133</v>
+      </c>
+      <c r="G50" t="s">
         <v>49</v>
       </c>
-      <c r="I49"/>
-      <c r="K49" t="s">
+      <c r="I50"/>
+      <c r="K50" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I50"/>
-    </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="I51"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>129</v>
       </c>
-      <c r="B51" t="s">
-        <v>40</v>
-      </c>
-      <c r="C51" t="s">
-        <v>17</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="B52" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" t="s">
         <v>122</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F52" t="s">
         <v>82</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G52" t="s">
         <v>46</v>
       </c>
-      <c r="I51"/>
-      <c r="K51" t="s">
+      <c r="I52"/>
+      <c r="K52" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I52"/>
-    </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="I53"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>157</v>
       </c>
-      <c r="B53" t="s">
-        <v>40</v>
-      </c>
-      <c r="C53" t="s">
-        <v>17</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="B54" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" t="s">
         <v>123</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F54" t="s">
         <v>150</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G54" t="s">
         <v>52</v>
       </c>
-      <c r="I53"/>
-      <c r="K53" t="s">
+      <c r="I54"/>
+      <c r="K54" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I54"/>
-    </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>155</v>
-      </c>
-      <c r="B55" t="s">
-        <v>31</v>
-      </c>
-      <c r="C55" t="s">
-        <v>17</v>
-      </c>
-      <c r="E55" t="s">
-        <v>123</v>
-      </c>
-      <c r="F55" t="s">
-        <v>151</v>
-      </c>
-      <c r="G55" t="s">
-        <v>152</v>
-      </c>
-      <c r="I55" t="s">
-        <v>153</v>
-      </c>
+      <c r="I55"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B56" t="s">
         <v>31</v>
@@ -1953,36 +1962,59 @@
         <v>151</v>
       </c>
       <c r="G56" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I56" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I57"/>
+      <c r="A57" t="s">
+        <v>156</v>
+      </c>
+      <c r="B57" t="s">
+        <v>31</v>
+      </c>
+      <c r="C57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" t="s">
+        <v>123</v>
+      </c>
+      <c r="F57" t="s">
+        <v>151</v>
+      </c>
+      <c r="G57" t="s">
+        <v>154</v>
+      </c>
+      <c r="I57" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="I58"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>128</v>
       </c>
-      <c r="B58" t="s">
-        <v>40</v>
-      </c>
-      <c r="C58" t="s">
-        <v>17</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="B59" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" t="s">
+        <v>17</v>
+      </c>
+      <c r="E59" t="s">
         <v>124</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F59" t="s">
         <v>125</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G59" t="s">
         <v>126</v>
       </c>
-      <c r="I58"/>
-      <c r="K58" s="3" t="s">
+      <c r="I59"/>
+      <c r="K59" s="3" t="s">
         <v>127</v>
       </c>
     </row>

</xml_diff>